<commit_message>
Com resultado de Leitura
</commit_message>
<xml_diff>
--- a/exemplo de requisição.xlsx
+++ b/exemplo de requisição.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t xml:space="preserve">Ação</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t xml:space="preserve">Ler FIFO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESPOSTA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">000000400000000000a34a47002f8b56a0afc105401e441d0000000000000089000000400000000080a5283c403c712300d8161980534d210000000000000034</t>
   </si>
 </sst>
 </file>
@@ -99,6 +105,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -199,15 +206,15 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="1" width="3.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="1" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -423,9 +430,13 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -486,7 +497,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>

</xml_diff>